<commit_message>
added BaseTest.java, LoginPage.java and NewArticleTest.java stubs
</commit_message>
<xml_diff>
--- a/manualTestCases.xlsx
+++ b/manualTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\exercisebackbase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363FBA44-879C-49A5-8B34-38E58BC7E018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0846E615-BC52-4380-BCC0-FA975074C223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42D77E7F-6EE1-4664-820D-BE5E5908B5A2}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{42D77E7F-6EE1-4664-820D-BE5E5908B5A2}"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD Articles" sheetId="1" r:id="rId1"/>
@@ -359,6 +359,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -368,65 +407,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -750,13 +750,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1953EAA-8500-4D8F-A620-0C54AD920B50}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
@@ -790,10 +790,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3">
@@ -805,15 +805,15 @@
       <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
@@ -823,13 +823,13 @@
       <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="3">
         <v>3</v>
       </c>
@@ -839,25 +839,25 @@
       <c r="E4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="3">
@@ -869,15 +869,15 @@
       <c r="E6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -887,35 +887,35 @@
       <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3">
@@ -927,15 +927,15 @@
       <c r="E10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="3">
         <v>2</v>
       </c>
@@ -945,13 +945,13 @@
       <c r="E11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="3">
         <v>3</v>
       </c>
@@ -961,13 +961,13 @@
       <c r="E12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="3">
         <v>4</v>
       </c>
@@ -977,25 +977,25 @@
       <c r="E13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="3">
@@ -1007,15 +1007,15 @@
       <c r="E15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="24" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="3">
         <v>2</v>
       </c>
@@ -1025,13 +1025,13 @@
       <c r="E16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="3">
         <v>3</v>
       </c>
@@ -1041,35 +1041,35 @@
       <c r="E17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="3">
@@ -1081,13 +1081,13 @@
       <c r="E20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="22"/>
       <c r="C21" s="3">
         <v>2</v>
       </c>
@@ -1097,11 +1097,11 @@
       <c r="E21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:8" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="3">
         <v>3</v>
       </c>
@@ -1111,29 +1111,29 @@
       <c r="E22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="F22" s="25"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="19"/>
+      <c r="F23" s="26"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="16"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="3">
@@ -1150,8 +1150,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="22"/>
       <c r="C26" s="3">
         <v>2</v>
       </c>
@@ -1164,8 +1164,8 @@
       <c r="F26" s="28"/>
     </row>
     <row r="27" spans="1:8" ht="118.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="3">
         <v>3</v>
       </c>
@@ -1178,38 +1178,21 @@
       <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="26">
+      <c r="A28" s="20"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="11">
         <v>4</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="11" t="s">
         <v>48</v>
       </c>
       <c r="F28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="G17:G19"/>
     <mergeCell ref="H17:H19"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="H7:H9"/>
@@ -1217,6 +1200,23 @@
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="F10:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>